<commit_message>
.done working on it for today
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,13 +421,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>value</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>world!</t>
         </is>

</xml_diff>